<commit_message>
Data Capturing bot completion
</commit_message>
<xml_diff>
--- a/Robot2_DataCapturing/customers.xlsx
+++ b/Robot2_DataCapturing/customers.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonidas Petrou\Desktop\Bots\Bot2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7812D967-FD3E-4DAC-9378-296F106BCD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2512,35 +2519,72 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri Light"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2548,7 +2592,7 @@
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2556,35 +2600,14 @@
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2592,7 +2615,7 @@
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2600,14 +2623,7 @@
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2615,22 +2631,14 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2638,14 +2646,35 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2658,175 +2687,188 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2836,6 +2878,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2861,7 +2918,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2896,15 +2953,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2920,17 +2968,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2946,105 +2988,129 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3093,7 +3159,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3126,26 +3192,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3178,23 +3227,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3336,37 +3368,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.4380952380952" customWidth="1"/>
+    <col min="2" max="2" width="11.552380952381" customWidth="1"/>
+    <col min="3" max="3" width="17.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="22.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="15.1047619047619" customWidth="1"/>
+    <col min="6" max="6" width="17.3333333333333" customWidth="1"/>
+    <col min="7" max="8" width="12.3333333333333" customWidth="1"/>
+    <col min="9" max="9" width="32.552380952381" customWidth="1"/>
+    <col min="10" max="10" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3398,7 +3425,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -3430,7 +3457,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3462,7 +3489,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -3494,7 +3521,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3526,7 +3553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -3558,7 +3585,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3590,7 +3617,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -3622,7 +3649,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -3654,7 +3681,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -3686,7 +3713,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -3718,7 +3745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -3750,7 +3777,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>110</v>
       </c>
@@ -3782,7 +3809,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -3814,7 +3841,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -3846,7 +3873,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -3878,7 +3905,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -3910,7 +3937,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>154</v>
       </c>
@@ -3942,7 +3969,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -3974,7 +4001,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>171</v>
       </c>
@@ -4006,7 +4033,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>180</v>
       </c>
@@ -4038,7 +4065,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>188</v>
       </c>
@@ -4070,7 +4097,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>197</v>
       </c>
@@ -4102,7 +4129,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>205</v>
       </c>
@@ -4134,7 +4161,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>214</v>
       </c>
@@ -4166,7 +4193,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>221</v>
       </c>
@@ -4198,7 +4225,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>230</v>
       </c>
@@ -4230,7 +4257,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
         <v>238</v>
       </c>
@@ -4262,7 +4289,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
         <v>247</v>
       </c>
@@ -4294,7 +4321,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>254</v>
       </c>
@@ -4326,7 +4353,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>263</v>
       </c>
@@ -4358,7 +4385,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>270</v>
       </c>
@@ -4390,7 +4417,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
         <v>278</v>
       </c>
@@ -4422,7 +4449,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
         <v>285</v>
       </c>
@@ -4454,7 +4481,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
         <v>293</v>
       </c>
@@ -4486,7 +4513,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
         <v>301</v>
       </c>
@@ -4518,7 +4545,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
         <v>309</v>
       </c>
@@ -4550,7 +4577,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
         <v>317</v>
       </c>
@@ -4582,7 +4609,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
         <v>326</v>
       </c>
@@ -4614,7 +4641,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
         <v>334</v>
       </c>
@@ -4646,7 +4673,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
         <v>343</v>
       </c>
@@ -4678,7 +4705,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
         <v>352</v>
       </c>
@@ -4710,7 +4737,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
         <v>360</v>
       </c>
@@ -4742,7 +4769,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
         <v>368</v>
       </c>
@@ -4774,7 +4801,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
         <v>376</v>
       </c>
@@ -4806,7 +4833,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
         <v>384</v>
       </c>
@@ -4838,7 +4865,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
         <v>393</v>
       </c>
@@ -4870,7 +4897,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
         <v>402</v>
       </c>
@@ -4902,7 +4929,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
         <v>409</v>
       </c>
@@ -4934,7 +4961,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
         <v>417</v>
       </c>
@@ -4966,7 +4993,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
         <v>426</v>
       </c>
@@ -4998,7 +5025,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
         <v>434</v>
       </c>
@@ -5030,7 +5057,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
         <v>441</v>
       </c>
@@ -5062,7 +5089,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
         <v>450</v>
       </c>
@@ -5094,7 +5121,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
         <v>458</v>
       </c>
@@ -5126,7 +5153,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -5158,7 +5185,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
         <v>474</v>
       </c>
@@ -5190,7 +5217,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
         <v>482</v>
       </c>
@@ -5222,7 +5249,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
         <v>489</v>
       </c>
@@ -5254,7 +5281,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
         <v>497</v>
       </c>
@@ -5286,7 +5313,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
         <v>506</v>
       </c>
@@ -5318,7 +5345,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
         <v>514</v>
       </c>
@@ -5350,7 +5377,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
         <v>521</v>
       </c>
@@ -5382,7 +5409,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
         <v>528</v>
       </c>
@@ -5414,7 +5441,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
         <v>535</v>
       </c>
@@ -5446,7 +5473,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
         <v>543</v>
       </c>
@@ -5478,7 +5505,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
         <v>550</v>
       </c>
@@ -5510,7 +5537,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
         <v>558</v>
       </c>
@@ -5542,7 +5569,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
         <v>566</v>
       </c>
@@ -5574,7 +5601,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
         <v>574</v>
       </c>
@@ -5606,7 +5633,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
         <v>583</v>
       </c>
@@ -5638,7 +5665,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
         <v>592</v>
       </c>
@@ -5670,7 +5697,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
         <v>600</v>
       </c>
@@ -5702,7 +5729,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
         <v>608</v>
       </c>
@@ -5734,7 +5761,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
         <v>616</v>
       </c>
@@ -5766,7 +5793,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
         <v>624</v>
       </c>
@@ -5798,7 +5825,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
         <v>632</v>
       </c>
@@ -5830,7 +5857,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
         <v>640</v>
       </c>
@@ -5862,7 +5889,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
         <v>648</v>
       </c>
@@ -5894,7 +5921,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
         <v>655</v>
       </c>
@@ -5926,7 +5953,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
         <v>663</v>
       </c>
@@ -5958,7 +5985,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
         <v>672</v>
       </c>
@@ -5990,7 +6017,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
         <v>679</v>
       </c>
@@ -6022,7 +6049,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
         <v>687</v>
       </c>
@@ -6054,7 +6081,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
         <v>695</v>
       </c>
@@ -6086,7 +6113,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
         <v>704</v>
       </c>
@@ -6118,7 +6145,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
         <v>712</v>
       </c>
@@ -6150,7 +6177,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
         <v>719</v>
       </c>
@@ -6182,7 +6209,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
         <v>727</v>
       </c>
@@ -6214,7 +6241,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
         <v>735</v>
       </c>
@@ -6246,7 +6273,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
         <v>743</v>
       </c>
@@ -6278,7 +6305,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
         <v>751</v>
       </c>
@@ -6310,7 +6337,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10">
       <c r="A93" t="s">
         <v>759</v>
       </c>
@@ -6342,7 +6369,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10">
       <c r="A94" t="s">
         <v>766</v>
       </c>
@@ -6374,7 +6401,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10">
       <c r="A95" t="s">
         <v>774</v>
       </c>
@@ -6406,7 +6433,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10">
       <c r="A96" t="s">
         <v>783</v>
       </c>
@@ -6438,7 +6465,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10">
       <c r="A97" t="s">
         <v>790</v>
       </c>
@@ -6470,7 +6497,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10">
       <c r="A98" t="s">
         <v>798</v>
       </c>
@@ -6502,7 +6529,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10">
       <c r="A99" t="s">
         <v>805</v>
       </c>
@@ -6534,7 +6561,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10">
       <c r="A100" t="s">
         <v>813</v>
       </c>
@@ -6566,7 +6593,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10">
       <c r="A101" t="s">
         <v>821</v>
       </c>
@@ -6600,5 +6627,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>